<commit_message>
Update FLMALS, make FMALN
worked on FLMALS, FLMAN, MALDIS, tables
</commit_message>
<xml_diff>
--- a/Architecture.xlsx
+++ b/Architecture.xlsx
@@ -9,22 +9,23 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12315" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="GroMALS" sheetId="1" r:id="rId1"/>
-    <sheet name="GroMALN" sheetId="2" r:id="rId2"/>
-    <sheet name="GroMALP" sheetId="5" r:id="rId3"/>
-    <sheet name="GroMALC" sheetId="4" r:id="rId4"/>
-    <sheet name="MALDIS" sheetId="6" r:id="rId5"/>
-    <sheet name="equations exploration" sheetId="3" r:id="rId6"/>
+    <sheet name="FLMALS" sheetId="1" r:id="rId1"/>
+    <sheet name="DAYLP" sheetId="7" r:id="rId2"/>
+    <sheet name="MALDIS" sheetId="6" r:id="rId3"/>
+    <sheet name="FLMALN" sheetId="2" r:id="rId4"/>
+    <sheet name="GroMALP" sheetId="5" r:id="rId5"/>
+    <sheet name="GroMALC" sheetId="4" r:id="rId6"/>
+    <sheet name="equations exploration" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="263">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -140,9 +141,6 @@
     <t>in broch, we have ~ 0.6 g/dm2</t>
   </si>
   <si>
-    <t>6 dm2 with 0.6 g per dm2 = 3.6 g</t>
-  </si>
-  <si>
     <t>m2/DM</t>
   </si>
   <si>
@@ -161,9 +159,6 @@
     <t>gN/m3</t>
   </si>
   <si>
-    <t>kn</t>
-  </si>
-  <si>
     <t>N:C ratio in structural mass</t>
   </si>
   <si>
@@ -209,12 +204,6 @@
     <t>(epsilon) erosion/mortality parameter macroalgae</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>day of year</t>
-  </si>
-  <si>
     <t>latitude (degrees)</t>
   </si>
   <si>
@@ -356,43 +345,475 @@
     <t>TIC</t>
   </si>
   <si>
-    <t>Hmax</t>
-  </si>
-  <si>
-    <t>Hmin</t>
-  </si>
-  <si>
     <t>DenMAL</t>
   </si>
   <si>
     <t>Maximum heigh MAL</t>
   </si>
   <si>
-    <t>Minimum height MAL</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
-    <t>g/m</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
-    <t>Length of MAL group</t>
-  </si>
-  <si>
     <t>linear density of macroalgae</t>
   </si>
   <si>
-    <t>POC1</t>
-  </si>
-  <si>
-    <t>PON1</t>
-  </si>
-  <si>
-    <t>POP1</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>daylengthd</t>
+  </si>
+  <si>
+    <t>daylengthp</t>
+  </si>
+  <si>
+    <t>daylengthm</t>
+  </si>
+  <si>
+    <t>length of current day</t>
+  </si>
+  <si>
+    <t>length of previous day</t>
+  </si>
+  <si>
+    <t>maximum length of day at this latitude</t>
+  </si>
+  <si>
+    <t>(d)</t>
+  </si>
+  <si>
+    <t>DCRatMALS</t>
+  </si>
+  <si>
+    <t>NCRatMALS</t>
+  </si>
+  <si>
+    <t>PCRatMALS</t>
+  </si>
+  <si>
+    <t>FrPOC1MALS</t>
+  </si>
+  <si>
+    <t>Surf</t>
+  </si>
+  <si>
+    <t>DELT</t>
+  </si>
+  <si>
+    <t>FrPOC2MALS</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m </t>
+  </si>
+  <si>
+    <t>dry mass to C content in MALS</t>
+  </si>
+  <si>
+    <t>N:C ratio in MALS</t>
+  </si>
+  <si>
+    <t>P:C ratio in MALS</t>
+  </si>
+  <si>
+    <t>fraction of MALS that goes to POC1 in decay</t>
+  </si>
+  <si>
+    <t>fraction of MALS that goes to POC2 in decay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horizontal surface area of a DELWAQ segment   </t>
+  </si>
+  <si>
+    <t>timestep for processes</t>
+  </si>
+  <si>
+    <t>depth of segment</t>
+  </si>
+  <si>
+    <t>0;</t>
+  </si>
+  <si>
+    <t>N;</t>
+  </si>
+  <si>
+    <t># output items for segments</t>
+  </si>
+  <si>
+    <t># input items for segments</t>
+  </si>
+  <si>
+    <t>MALSM2</t>
+  </si>
+  <si>
+    <t>LimBioMALS</t>
+  </si>
+  <si>
+    <t>LimPhoMALS</t>
+  </si>
+  <si>
+    <t>LimTemMALS</t>
+  </si>
+  <si>
+    <t>biomass limitation MALS</t>
+  </si>
+  <si>
+    <t>photoperiod limitation MALS</t>
+  </si>
+  <si>
+    <t>temperature limitation MALS</t>
+  </si>
+  <si>
+    <t>(gDM/m3/d)</t>
+  </si>
+  <si>
+    <t>(gN/m3/d)</t>
+  </si>
+  <si>
+    <t>(gP/m3/d)</t>
+  </si>
+  <si>
+    <t>(gC/m3/d)</t>
+  </si>
+  <si>
+    <t>dPrPOC1MAL</t>
+  </si>
+  <si>
+    <t>POC1 production MALS</t>
+  </si>
+  <si>
+    <t>dPrPOC2MAL</t>
+  </si>
+  <si>
+    <t>POC2 production MALS</t>
+  </si>
+  <si>
+    <t>dPrPON1MAL</t>
+  </si>
+  <si>
+    <t>PON1 production MALS</t>
+  </si>
+  <si>
+    <t>dPrPON2MAL</t>
+  </si>
+  <si>
+    <t>PON2 production MALS</t>
+  </si>
+  <si>
+    <t>dPrPOP1MAL</t>
+  </si>
+  <si>
+    <t>POP1 production MALS</t>
+  </si>
+  <si>
+    <t>dPrPOP2MAL</t>
+  </si>
+  <si>
+    <t>POP2 production MALS</t>
+  </si>
+  <si>
+    <t>dMALSOXY</t>
+  </si>
+  <si>
+    <t>oxygen production MALS</t>
+  </si>
+  <si>
+    <t>(gO/m3/d)</t>
+  </si>
+  <si>
+    <t>FrMALS</t>
+  </si>
+  <si>
+    <t>Fraction of bottom layer MALS in this segment</t>
+  </si>
+  <si>
+    <t>FlMALS</t>
+  </si>
+  <si>
+    <t>FLMALS</t>
+  </si>
+  <si>
+    <t># output items for exchanges</t>
+  </si>
+  <si>
+    <t># fluxes</t>
+  </si>
+  <si>
+    <t># input items for exchanges</t>
+  </si>
+  <si>
+    <t>Flux calculation for Macroalgae Structural Mass</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>26;</t>
+  </si>
+  <si>
+    <t>HmaxMAL</t>
+  </si>
+  <si>
+    <t>g/m3</t>
+  </si>
+  <si>
+    <t>TotalDepth</t>
+  </si>
+  <si>
+    <t>LocalDepth</t>
+  </si>
+  <si>
+    <t>total depth of water column</t>
+  </si>
+  <si>
+    <t>depth from water syrface to bottom of segment</t>
+  </si>
+  <si>
+    <t>BmLayMAL</t>
+  </si>
+  <si>
+    <t>HactMAL</t>
+  </si>
+  <si>
+    <t>Biomass of MAL in segment</t>
+  </si>
+  <si>
+    <t>Actual length of macroalgae</t>
+  </si>
+  <si>
+    <t>FrBmMALS</t>
+  </si>
+  <si>
+    <t>Fraction biomass per layer macroalgae structural</t>
+  </si>
+  <si>
+    <t>10;</t>
+  </si>
+  <si>
+    <t>MALNM2</t>
+  </si>
+  <si>
+    <t>MALPM2</t>
+  </si>
+  <si>
+    <t>MALCM2</t>
+  </si>
+  <si>
+    <t>macroalgae structural in segment</t>
+  </si>
+  <si>
+    <t>macroalgae N storage in segment</t>
+  </si>
+  <si>
+    <t>macroalgae P storage in segment</t>
+  </si>
+  <si>
+    <t>macroalgae C storage in segment</t>
+  </si>
+  <si>
+    <t>14;</t>
+  </si>
+  <si>
+    <t>7;</t>
+  </si>
+  <si>
+    <t>REAL(4)</t>
+  </si>
+  <si>
+    <t>LocGroS</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>local growth of MALS</t>
+  </si>
+  <si>
+    <t>LocGroN</t>
+  </si>
+  <si>
+    <t>local growth of MALN</t>
+  </si>
+  <si>
+    <t>LocGroP</t>
+  </si>
+  <si>
+    <t>local growth of MALP</t>
+  </si>
+  <si>
+    <t>LocGroC</t>
+  </si>
+  <si>
+    <t>local growth of MALC</t>
+  </si>
+  <si>
+    <t>13;</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>DAYLP</t>
+  </si>
+  <si>
+    <t>DaylengthP</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>RefDay</t>
+  </si>
+  <si>
+    <t>AuxSys</t>
+  </si>
+  <si>
+    <t>ITIME</t>
+  </si>
+  <si>
+    <t>daylength default definition</t>
+  </si>
+  <si>
+    <t>daylength of previous day</t>
+  </si>
+  <si>
+    <t>maximum daylength at this latitude</t>
+  </si>
+  <si>
+    <t>(scu)</t>
+  </si>
+  <si>
+    <t>latitude of study area</t>
+  </si>
+  <si>
+    <t>(degrees)</t>
+  </si>
+  <si>
+    <t>daynumber of reference day simulation</t>
+  </si>
+  <si>
+    <t>ratio between days and system clock</t>
+  </si>
+  <si>
+    <t>(scu/d)</t>
+  </si>
+  <si>
+    <t>3;</t>
+  </si>
+  <si>
+    <t>4;</t>
+  </si>
+  <si>
+    <t># stoichiometry lines</t>
+  </si>
+  <si>
+    <t># stoichiometry lines dispersion arrays</t>
+  </si>
+  <si>
+    <t># stoichiometry lines velocity arrays</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>FlMALN</t>
+  </si>
+  <si>
+    <t>FLMALN</t>
+  </si>
+  <si>
+    <t>Flux calculation for Macroalgae Nitrogen storage</t>
+  </si>
+  <si>
+    <t>LocUpN</t>
+  </si>
+  <si>
+    <t>Local N uptake flux</t>
+  </si>
+  <si>
+    <t>dUpMALNO3</t>
+  </si>
+  <si>
+    <t>NO3 uptake by Macroalgae nitrogen storage</t>
+  </si>
+  <si>
+    <t>NH4 uptake by Macroalgae nitrogen storage</t>
+  </si>
+  <si>
+    <t>dUpMALNH4</t>
+  </si>
+  <si>
+    <t>2;</t>
+  </si>
+  <si>
+    <t>CDRatMALS</t>
+  </si>
+  <si>
+    <t>C:DM ratio in structural mass</t>
+  </si>
+  <si>
+    <t>gC/gDN</t>
+  </si>
+  <si>
+    <t>PMSA( IPNT(2) )</t>
+  </si>
+  <si>
+    <t>PMSA( IPNT(3) )</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>(gN/gDM)</t>
+  </si>
+  <si>
+    <t>(gN/m3)</t>
+  </si>
+  <si>
+    <t>Fraction of MALS in this segment</t>
+  </si>
+  <si>
+    <t>(-)</t>
+  </si>
+  <si>
+    <t>minimal N in nitrogen storage</t>
+  </si>
+  <si>
+    <t>maximum N in nitrogen storage</t>
+  </si>
+  <si>
+    <t>Carbon to dry matter ratio in MALS</t>
+  </si>
+  <si>
+    <t>(gC/gDM)</t>
+  </si>
+  <si>
+    <t>Nitrogen to carbon ratio in MALS</t>
+  </si>
+  <si>
+    <t>(gN/gC)</t>
+  </si>
+  <si>
+    <t>horizontal surface area of a DELWAQ segment</t>
+  </si>
+  <si>
+    <t>(m2)</t>
+  </si>
+  <si>
+    <t>(m)</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>LimVel</t>
+  </si>
+  <si>
+    <t>velocity limitation</t>
   </si>
 </sst>
 </file>
@@ -467,11 +888,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,8 +900,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,11 +1215,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210637664"/>
-        <c:axId val="210631784"/>
+        <c:axId val="421215808"/>
+        <c:axId val="421218944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210637664"/>
+        <c:axId val="421215808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,12 +1229,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210631784"/>
+        <c:crossAx val="421218944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210631784"/>
+        <c:axId val="421218944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -826,7 +1245,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="210637664"/>
+        <c:crossAx val="421215808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1169,395 +1588,1166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5">
         <v>-999</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="6">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5">
         <v>-999</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6">
-        <f>6*0.6</f>
-        <v>3.5999999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="6">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6">
         <v>-999</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="7">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" s="8">
         <v>-999</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="C9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="6">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5">
         <v>0.01</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="C11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E11" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5">
+        <v>15</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="5">
+        <v>0.1085</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="5">
+        <f>6*G5</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="5">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+    </row>
+    <row r="22" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="8" t="e">
+        <f>0.3/G5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="8">
+        <v>0.75</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="E37" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="6">
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="8"/>
+      <c r="C38" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+      <c r="B46" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" s="9"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+      <c r="B47" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5">
         <v>-999</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="6">
-        <v>15</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="6" t="s">
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B8">
+        <v>86400</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
+        <v>222</v>
+      </c>
+      <c r="E8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>215</v>
+      </c>
+      <c r="E11" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="6">
-        <v>0.1085</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="6" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>216</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="6">
-        <v>0.03</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6">
-        <f>6*F3</f>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="6" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>217</v>
+      </c>
+      <c r="E13" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="6">
-        <v>0.85</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="7">
-        <f>0.3/F3</f>
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-    </row>
-    <row r="20" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>122</v>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1565,279 +2755,1228 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D31" sqref="D31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>-999</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="5">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="5">
+        <v>100</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:7" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>232</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>123</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
         <v>-999</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
         <f>6*0.6</f>
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B7" s="6">
+        <v>-999</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="7">
-        <v>-999</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="F13" s="5">
+        <f>4*H13*0.001</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B14" s="5">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="6">
-        <f>4*F11*0.001</f>
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="F14" s="5">
         <f>0.00014*24/0.6</f>
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-999</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="E15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="5">
+        <v>-999</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="E16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="8">
         <v>-999</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="7">
-        <v>0.03</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="C17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="8">
+        <v>-999</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>235</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="B37" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C38" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C39" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C40" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C41" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C42" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>241</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C44" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C45" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C48" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>122</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C49" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C50" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="C51" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>197</v>
+      </c>
+      <c r="C52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52" t="s">
+        <v>11</v>
+      </c>
+      <c r="G52" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" t="s">
+        <v>199</v>
+      </c>
+      <c r="E53" t="s">
+        <v>246</v>
+      </c>
+      <c r="F53" t="s">
+        <v>229</v>
+      </c>
+      <c r="G53" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>197</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" t="s">
+        <v>199</v>
+      </c>
+      <c r="E54" t="s">
+        <v>246</v>
+      </c>
+      <c r="F54" t="s">
+        <v>230</v>
+      </c>
+      <c r="G54" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>197</v>
+      </c>
+      <c r="C55" t="s">
+        <v>185</v>
+      </c>
+      <c r="D55" t="s">
+        <v>199</v>
+      </c>
+      <c r="E55" t="s">
+        <v>246</v>
+      </c>
+      <c r="F55" t="s">
+        <v>249</v>
+      </c>
+      <c r="G55" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>197</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>199</v>
+      </c>
+      <c r="E56" t="s">
+        <v>246</v>
+      </c>
+      <c r="F56" t="s">
+        <v>251</v>
+      </c>
+      <c r="G56" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>197</v>
+      </c>
+      <c r="C57" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" t="s">
+        <v>199</v>
+      </c>
+      <c r="E57" t="s">
+        <v>246</v>
+      </c>
+      <c r="F57" t="s">
+        <v>252</v>
+      </c>
+      <c r="G57" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>197</v>
+      </c>
+      <c r="C58" t="s">
+        <v>241</v>
+      </c>
+      <c r="D58" t="s">
+        <v>199</v>
+      </c>
+      <c r="E58" t="s">
+        <v>246</v>
+      </c>
+      <c r="F58" t="s">
+        <v>253</v>
+      </c>
+      <c r="G58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>197</v>
+      </c>
+      <c r="C59" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" t="s">
+        <v>199</v>
+      </c>
+      <c r="E59" t="s">
+        <v>246</v>
+      </c>
+      <c r="F59" t="s">
+        <v>255</v>
+      </c>
+      <c r="G59" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>197</v>
+      </c>
+      <c r="C61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" t="s">
+        <v>53</v>
+      </c>
+      <c r="D62" t="s">
+        <v>199</v>
+      </c>
+      <c r="E62" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" t="s">
+        <v>199</v>
+      </c>
+      <c r="E64" t="s">
+        <v>246</v>
+      </c>
+      <c r="F64" t="s">
+        <v>257</v>
+      </c>
+      <c r="G64" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" t="s">
+        <v>123</v>
+      </c>
+      <c r="D65" t="s">
+        <v>199</v>
+      </c>
+      <c r="E65" t="s">
+        <v>246</v>
+      </c>
+      <c r="F65" t="s">
+        <v>133</v>
+      </c>
+      <c r="G65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C66" t="s">
+        <v>78</v>
+      </c>
+      <c r="D66" t="s">
+        <v>199</v>
+      </c>
+      <c r="E66" t="s">
+        <v>246</v>
+      </c>
+      <c r="F66" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" t="s">
+        <v>259</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -1854,36 +3993,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
+      <c r="A3" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -1891,16 +4030,16 @@
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>-999</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
         <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1909,191 +4048,191 @@
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>-999</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
         <f>6*0.6</f>
         <v>3.5999999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>70</v>
+      <c r="A5" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="6">
+        <v>67</v>
+      </c>
+      <c r="D5" s="5">
         <v>-999</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="A6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.01</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>47</v>
+      <c r="A8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.01</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>73</v>
+      <c r="A9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.2</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="6">
+      <c r="C10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="5">
         <f>4*F10*0.001</f>
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="A11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="5">
         <f>0.00014*24/0.6</f>
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>0.03</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -2110,36 +4249,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
+      <c r="A3" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -2147,131 +4286,131 @@
       <c r="C3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>-999</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5">
         <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>-999</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="A5" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.01</v>
       </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>83</v>
+      <c r="A7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="6">
+        <v>56</v>
+      </c>
+      <c r="D7" s="5">
         <v>-999</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="B8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="5">
         <v>15</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="A9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="5">
         <f>285</f>
         <v>285</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="A10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="5">
         <f>290</f>
         <v>290</v>
       </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="D11">
         <f>1694.4-273</f>
@@ -2279,173 +4418,173 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="A12" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="5">
         <f>25924</f>
         <v>25924</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="A13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="5">
         <v>27774</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" s="6">
+      <c r="A14" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="5">
         <v>11033</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D15" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B16" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="6">
-        <v>-999</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C17" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D17" s="5">
         <f>0.0000375*(1/F3)*24</f>
         <v>1.5E-3</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D18" s="7">
+      <c r="A18" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="6">
         <v>200</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="A19" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>108</v>
+      <c r="A23" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
-        <v>109</v>
+      <c r="A24" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="B24">
         <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="9" t="s">
         <v>10</v>
       </c>
       <c r="B25">
@@ -2457,223 +4596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="6">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="6">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="6">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="7">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D11" s="6">
-        <v>-999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="10"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="6">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D356"/>
   <sheetViews>
@@ -2685,16 +4608,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B1">
         <v>0.1085</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2714,7 +4637,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B3">
         <v>6</v>

</xml_diff>